<commit_message>
Updated metadata spreadsheet and installer.
git-svn-id: http://Marc-PC/svn/Full@583 85f15e0e-5137-b144-a863-98bd542365a3
</commit_message>
<xml_diff>
--- a/trunk/Century-succession/trunk/deploy/docs/Century-succession-log-metadata.xlsx
+++ b/trunk/Century-succession/trunk/deploy/docs/Century-succession-log-metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="18075" windowHeight="7935"/>
+    <workbookView xWindow="840" yWindow="4515" windowWidth="18075" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="117">
   <si>
     <t>Time</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Net mineralization from the surface metabolic pool (g N m-2 yr-1)</t>
   </si>
   <si>
-    <t>Carbon that is lost due to volitization (g C m-2 yr-1)</t>
-  </si>
-  <si>
     <t>Nitrogen that is transported out of the system via water (g N m-2 yr-1)</t>
   </si>
   <si>
@@ -314,23 +311,68 @@
     <t>Nitrogen in live wood or coarse roots (g N m-2)</t>
   </si>
   <si>
-    <t>Net minerization from the SOM1-surface (g N m-2 yr-1)</t>
+    <t xml:space="preserve"> LitterfallC</t>
   </si>
   <si>
-    <t>Net minerization from the SOM1-soil (g N m-2 yr-1)</t>
+    <t xml:space="preserve"> FireCEfflux</t>
   </si>
   <si>
-    <t>Net minerization from the SOM2 (g N m-2 yr-1)</t>
+    <t xml:space="preserve"> FireNEfflux</t>
   </si>
   <si>
-    <t>Net minerization from the SOM3 (g N m-2 yr-1)</t>
+    <t>Carbon that is lost due to volatilization during fire (g C m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Nitrogen that is lost due to volatization during fire (g C m-2 yr-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nuptake</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nresorbed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TotalSoilN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nvol</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avgfrassC</t>
+  </si>
+  <si>
+    <t>Nitrogen that is taken up by the vegetation (g C m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Nitrogen that is resorbed/retranslocated by the vegetation (g C m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Nitrogen in soil (g N m-2)</t>
+  </si>
+  <si>
+    <t>Nitrogen that is lost due to volatilization, excludes fire (g C m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Carbon in insect frass (g C m-2)</t>
+  </si>
+  <si>
+    <t>Net  mineralization from the SOM1-surface (g N m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Net  mineralization from the SOM1-soil (g N m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Net  mineralization from the SOM2 (g N m-2 yr-1)</t>
+  </si>
+  <si>
+    <t>Net mineralization from the SOM3 (g N m-2 yr-1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,6 +906,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -942,6 +989,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -976,6 +1024,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1151,20 +1200,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B45" sqref="B42:B45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1221,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1180,7 +1229,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1245,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1204,7 +1253,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1261,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1269,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1228,15 +1277,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1244,7 +1293,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1252,7 +1301,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1260,7 +1309,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1268,7 +1317,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1325,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1284,7 +1333,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1341,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1300,15 +1349,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1316,7 +1365,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1324,7 +1373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1332,7 +1381,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1340,7 +1389,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1348,7 +1397,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1356,7 +1405,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1364,103 +1413,103 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1468,7 +1517,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1476,76 +1525,124 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1554,19 +1651,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1809,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:48">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1858,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:48">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2004,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:48">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2150,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:48">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2296,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:48">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2442,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:48">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2588,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:48">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2734,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:48">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2880,7 +2977,7 @@
         <v>54.215000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:48">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -3026,7 +3123,7 @@
         <v>36.564999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:48">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3172,7 +3269,7 @@
         <v>28.629000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:48">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3318,7 +3415,7 @@
         <v>4.9269999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:48">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -3464,7 +3561,7 @@
         <v>2.8180000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:48">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -3610,7 +3707,7 @@
         <v>8.3030000000000008</v>
       </c>
     </row>
-    <row r="15" spans="1:48">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -3756,7 +3853,7 @@
         <v>5.5060000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:48">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -3902,7 +3999,7 @@
         <v>87.757000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:48">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -4048,7 +4145,7 @@
         <v>55.204999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:48">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -4194,7 +4291,7 @@
         <v>30.658999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:48">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -4340,7 +4437,7 @@
         <v>8.3089999999999993</v>
       </c>
     </row>
-    <row r="20" spans="1:48">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -4486,7 +4583,7 @@
         <v>4.0469999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:48">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -4632,7 +4729,7 @@
         <v>7.6790000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:48">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -4778,7 +4875,7 @@
         <v>924.25599999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:48">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>15</v>
       </c>
@@ -4924,7 +5021,7 @@
         <v>164.34299999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:48">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -5070,7 +5167,7 @@
         <v>85.275000000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:48">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
@@ -5216,7 +5313,7 @@
         <v>81.39</v>
       </c>
     </row>
-    <row r="26" spans="1:48">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>15</v>
       </c>
@@ -5362,7 +5459,7 @@
         <v>6.9480000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:48">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15</v>
       </c>
@@ -5508,7 +5605,7 @@
         <v>3.68</v>
       </c>
     </row>
-    <row r="28" spans="1:48">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>15</v>
       </c>
@@ -5654,7 +5751,7 @@
         <v>8.6620000000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:48">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -5800,7 +5897,7 @@
         <v>1303.163</v>
       </c>
     </row>
-    <row r="30" spans="1:48">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -5946,7 +6043,7 @@
         <v>74.870999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:48">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20</v>
       </c>
@@ -6092,7 +6189,7 @@
         <v>37.847999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:48">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20</v>
       </c>
@@ -6238,7 +6335,7 @@
         <v>28.927</v>
       </c>
     </row>
-    <row r="33" spans="1:48">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
@@ -6384,7 +6481,7 @@
         <v>4.6669999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:48">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
@@ -6530,7 +6627,7 @@
         <v>3.133</v>
       </c>
     </row>
-    <row r="35" spans="1:48">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20</v>
       </c>
@@ -6676,7 +6773,7 @@
         <v>3.5569999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:48">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20</v>
       </c>
@@ -6822,7 +6919,7 @@
         <v>15.824</v>
       </c>
     </row>
-    <row r="37" spans="1:48">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>25</v>
       </c>
@@ -6968,7 +7065,7 @@
         <v>70.369</v>
       </c>
     </row>
-    <row r="38" spans="1:48">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>25</v>
       </c>
@@ -7114,7 +7211,7 @@
         <v>24.634</v>
       </c>
     </row>
-    <row r="39" spans="1:48">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>25</v>
       </c>
@@ -7260,7 +7357,7 @@
         <v>30.01</v>
       </c>
     </row>
-    <row r="40" spans="1:48">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>25</v>
       </c>
@@ -7406,7 +7503,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="41" spans="1:48">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>25</v>
       </c>
@@ -7552,7 +7649,7 @@
         <v>2.871</v>
       </c>
     </row>
-    <row r="42" spans="1:48">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>25</v>
       </c>
@@ -7698,7 +7795,7 @@
         <v>5.5380000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:48">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>25</v>
       </c>
@@ -7844,7 +7941,7 @@
         <v>94.650999999999996</v>
       </c>
     </row>
-    <row r="44" spans="1:48">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>30</v>
       </c>
@@ -7990,7 +8087,7 @@
         <v>222.267</v>
       </c>
     </row>
-    <row r="45" spans="1:48">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>30</v>
       </c>
@@ -8136,7 +8233,7 @@
         <v>145.01400000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:48">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>30</v>
       </c>
@@ -8282,7 +8379,7 @@
         <v>74.266999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:48">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>30</v>
       </c>
@@ -8428,7 +8525,7 @@
         <v>19.367000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:48">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>30</v>
       </c>
@@ -8574,7 +8671,7 @@
         <v>7.7450000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:48">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>30</v>
       </c>
@@ -8720,7 +8817,7 @@
         <v>17.027000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:48">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>30</v>
       </c>
@@ -8866,7 +8963,7 @@
         <v>186.48599999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:48">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>35</v>
       </c>
@@ -9012,7 +9109,7 @@
         <v>156.73599999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:48">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>35</v>
       </c>
@@ -9158,7 +9255,7 @@
         <v>103.617</v>
       </c>
     </row>
-    <row r="53" spans="1:48">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>35</v>
       </c>
@@ -9304,7 +9401,7 @@
         <v>72.02</v>
       </c>
     </row>
-    <row r="54" spans="1:48">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>35</v>
       </c>
@@ -9450,7 +9547,7 @@
         <v>17.443000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:48">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>35</v>
       </c>
@@ -9596,7 +9693,7 @@
         <v>4.4290000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:48">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>35</v>
       </c>
@@ -9742,7 +9839,7 @@
         <v>14.456</v>
       </c>
     </row>
-    <row r="57" spans="1:48">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>35</v>
       </c>
@@ -9888,7 +9985,7 @@
         <v>295.91899999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:48">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>40</v>
       </c>
@@ -10034,7 +10131,7 @@
         <v>67.135999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:48">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>40</v>
       </c>
@@ -10180,7 +10277,7 @@
         <v>50.116</v>
       </c>
     </row>
-    <row r="60" spans="1:48">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>40</v>
       </c>
@@ -10326,7 +10423,7 @@
         <v>33.981999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:48">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>40</v>
       </c>
@@ -10472,7 +10569,7 @@
         <v>5.6020000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:48">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>40</v>
       </c>
@@ -10618,7 +10715,7 @@
         <v>3.7879999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:48">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>40</v>
       </c>
@@ -10764,7 +10861,7 @@
         <v>8.6389999999999993</v>
       </c>
     </row>
-    <row r="64" spans="1:48">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>40</v>
       </c>
@@ -10910,7 +11007,7 @@
         <v>16.407</v>
       </c>
     </row>
-    <row r="65" spans="1:48">
+    <row r="65" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>45</v>
       </c>
@@ -11056,7 +11153,7 @@
         <v>63.774999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:48">
+    <row r="66" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>45</v>
       </c>
@@ -11202,7 +11299,7 @@
         <v>31.736000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:48">
+    <row r="67" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>45</v>
       </c>
@@ -11348,7 +11445,7 @@
         <v>51.192999999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:48">
+    <row r="68" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>45</v>
       </c>
@@ -11494,7 +11591,7 @@
         <v>10.516999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:48">
+    <row r="69" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>45</v>
       </c>
@@ -11640,7 +11737,7 @@
         <v>4.8330000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:48">
+    <row r="70" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>45</v>
       </c>
@@ -11786,7 +11883,7 @@
         <v>11.337</v>
       </c>
     </row>
-    <row r="71" spans="1:48">
+    <row r="71" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>45</v>
       </c>
@@ -11932,7 +12029,7 @@
         <v>3.9089999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:48">
+    <row r="72" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>50</v>
       </c>
@@ -12078,7 +12175,7 @@
         <v>38.225000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:48">
+    <row r="73" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>50</v>
       </c>
@@ -12224,7 +12321,7 @@
         <v>31.620999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:48">
+    <row r="74" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>50</v>
       </c>
@@ -12370,7 +12467,7 @@
         <v>31.350999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:48">
+    <row r="75" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>50</v>
       </c>
@@ -12516,7 +12613,7 @@
         <v>8.4359999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:48">
+    <row r="76" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>50</v>
       </c>
@@ -12662,7 +12759,7 @@
         <v>4.8230000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:48">
+    <row r="77" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>50</v>
       </c>
@@ -12808,7 +12905,7 @@
         <v>5.6989999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:48">
+    <row r="78" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>50</v>
       </c>
@@ -12954,7 +13051,7 @@
         <v>23.117000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:48">
+    <row r="79" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>55</v>
       </c>
@@ -13100,7 +13197,7 @@
         <v>129.989</v>
       </c>
     </row>
-    <row r="80" spans="1:48">
+    <row r="80" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>55</v>
       </c>
@@ -13246,7 +13343,7 @@
         <v>72.778999999999996</v>
       </c>
     </row>
-    <row r="81" spans="1:48">
+    <row r="81" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>55</v>
       </c>
@@ -13392,7 +13489,7 @@
         <v>72.078999999999994</v>
       </c>
     </row>
-    <row r="82" spans="1:48">
+    <row r="82" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>55</v>
       </c>
@@ -13538,7 +13635,7 @@
         <v>11.01</v>
       </c>
     </row>
-    <row r="83" spans="1:48">
+    <row r="83" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>55</v>
       </c>
@@ -13684,7 +13781,7 @@
         <v>14.154</v>
       </c>
     </row>
-    <row r="84" spans="1:48">
+    <row r="84" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>55</v>
       </c>
@@ -13830,7 +13927,7 @@
         <v>10.302</v>
       </c>
     </row>
-    <row r="85" spans="1:48">
+    <row r="85" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>55</v>
       </c>
@@ -13976,7 +14073,7 @@
         <v>442.65300000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:48">
+    <row r="86" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>60</v>
       </c>
@@ -14122,7 +14219,7 @@
         <v>37.264000000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:48">
+    <row r="87" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>60</v>
       </c>
@@ -14268,7 +14365,7 @@
         <v>38.320999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:48">
+    <row r="88" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>60</v>
       </c>
@@ -14414,7 +14511,7 @@
         <v>26.256</v>
       </c>
     </row>
-    <row r="89" spans="1:48">
+    <row r="89" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>60</v>
       </c>
@@ -14560,7 +14657,7 @@
         <v>6.34</v>
       </c>
     </row>
-    <row r="90" spans="1:48">
+    <row r="90" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>60</v>
       </c>
@@ -14706,7 +14803,7 @@
         <v>3.4460000000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:48">
+    <row r="91" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>60</v>
       </c>
@@ -14852,7 +14949,7 @@
         <v>5.4409999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:48">
+    <row r="92" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>60</v>
       </c>
@@ -14998,7 +15095,7 @@
         <v>0.89300000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:48">
+    <row r="93" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>65</v>
       </c>
@@ -15144,7 +15241,7 @@
         <v>32.537999999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:48">
+    <row r="94" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>65</v>
       </c>
@@ -15290,7 +15387,7 @@
         <v>52.35</v>
       </c>
     </row>
-    <row r="95" spans="1:48">
+    <row r="95" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>65</v>
       </c>
@@ -15436,7 +15533,7 @@
         <v>15.839</v>
       </c>
     </row>
-    <row r="96" spans="1:48">
+    <row r="96" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>65</v>
       </c>
@@ -15582,7 +15679,7 @@
         <v>7.048</v>
       </c>
     </row>
-    <row r="97" spans="1:48">
+    <row r="97" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>65</v>
       </c>
@@ -15728,7 +15825,7 @@
         <v>3.6030000000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:48">
+    <row r="98" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>65</v>
       </c>
@@ -15874,7 +15971,7 @@
         <v>5.5720000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:48">
+    <row r="99" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>65</v>
       </c>
@@ -16020,7 +16117,7 @@
         <v>716.92700000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:48">
+    <row r="100" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>70</v>
       </c>
@@ -16166,7 +16263,7 @@
         <v>90.075000000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:48">
+    <row r="101" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>70</v>
       </c>
@@ -16312,7 +16409,7 @@
         <v>40.384</v>
       </c>
     </row>
-    <row r="102" spans="1:48">
+    <row r="102" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>70</v>
       </c>
@@ -16458,7 +16555,7 @@
         <v>31.512</v>
       </c>
     </row>
-    <row r="103" spans="1:48">
+    <row r="103" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>70</v>
       </c>
@@ -16604,7 +16701,7 @@
         <v>9.766</v>
       </c>
     </row>
-    <row r="104" spans="1:48">
+    <row r="104" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>70</v>
       </c>
@@ -16750,7 +16847,7 @@
         <v>3.544</v>
       </c>
     </row>
-    <row r="105" spans="1:48">
+    <row r="105" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>70</v>
       </c>
@@ -16896,7 +16993,7 @@
         <v>7.97</v>
       </c>
     </row>
-    <row r="106" spans="1:48">
+    <row r="106" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>70</v>
       </c>
@@ -17042,7 +17139,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="107" spans="1:48">
+    <row r="107" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>75</v>
       </c>
@@ -17188,7 +17285,7 @@
         <v>99.397999999999996</v>
       </c>
     </row>
-    <row r="108" spans="1:48">
+    <row r="108" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>75</v>
       </c>
@@ -17334,7 +17431,7 @@
         <v>86.858000000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:48">
+    <row r="109" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>75</v>
       </c>
@@ -17480,7 +17577,7 @@
         <v>96.775000000000006</v>
       </c>
     </row>
-    <row r="110" spans="1:48">
+    <row r="110" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>75</v>
       </c>
@@ -17626,7 +17723,7 @@
         <v>9.0990000000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:48">
+    <row r="111" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>75</v>
       </c>
@@ -17772,7 +17869,7 @@
         <v>5.1459999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:48">
+    <row r="112" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>75</v>
       </c>
@@ -17918,7 +18015,7 @@
         <v>14.215</v>
       </c>
     </row>
-    <row r="113" spans="1:48">
+    <row r="113" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>75</v>
       </c>
@@ -18064,7 +18161,7 @@
         <v>78.709000000000003</v>
       </c>
     </row>
-    <row r="114" spans="1:48">
+    <row r="114" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>80</v>
       </c>
@@ -18210,7 +18307,7 @@
         <v>190.77799999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:48">
+    <row r="115" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>80</v>
       </c>
@@ -18356,7 +18453,7 @@
         <v>144.94999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:48">
+    <row r="116" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>80</v>
       </c>
@@ -18502,7 +18599,7 @@
         <v>97.427999999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:48">
+    <row r="117" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>80</v>
       </c>
@@ -18648,7 +18745,7 @@
         <v>20.893999999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:48">
+    <row r="118" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>80</v>
       </c>
@@ -18794,7 +18891,7 @@
         <v>5.2149999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:48">
+    <row r="119" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>80</v>
       </c>
@@ -18940,7 +19037,7 @@
         <v>11.071</v>
       </c>
     </row>
-    <row r="120" spans="1:48">
+    <row r="120" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>80</v>
       </c>
@@ -19086,7 +19183,7 @@
         <v>490.63600000000002</v>
       </c>
     </row>
-    <row r="121" spans="1:48">
+    <row r="121" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>85</v>
       </c>
@@ -19232,7 +19329,7 @@
         <v>232.78399999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:48">
+    <row r="122" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>85</v>
       </c>
@@ -19378,7 +19475,7 @@
         <v>284.29500000000002</v>
       </c>
     </row>
-    <row r="123" spans="1:48">
+    <row r="123" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>85</v>
       </c>
@@ -19524,7 +19621,7 @@
         <v>124.498</v>
       </c>
     </row>
-    <row r="124" spans="1:48">
+    <row r="124" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>85</v>
       </c>
@@ -19670,7 +19767,7 @@
         <v>29.452000000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:48">
+    <row r="125" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>85</v>
       </c>
@@ -19816,7 +19913,7 @@
         <v>11.753</v>
       </c>
     </row>
-    <row r="126" spans="1:48">
+    <row r="126" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>85</v>
       </c>
@@ -19962,7 +20059,7 @@
         <v>18.715</v>
       </c>
     </row>
-    <row r="127" spans="1:48">
+    <row r="127" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>85</v>
       </c>
@@ -20108,7 +20205,7 @@
         <v>654.03899999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:48">
+    <row r="128" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>90</v>
       </c>
@@ -20254,7 +20351,7 @@
         <v>35.570999999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:48">
+    <row r="129" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>90</v>
       </c>
@@ -20400,7 +20497,7 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="130" spans="1:48">
+    <row r="130" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>90</v>
       </c>
@@ -20546,7 +20643,7 @@
         <v>21.617000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:48">
+    <row r="131" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>90</v>
       </c>
@@ -20692,7 +20789,7 @@
         <v>5.577</v>
       </c>
     </row>
-    <row r="132" spans="1:48">
+    <row r="132" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>90</v>
       </c>
@@ -20838,7 +20935,7 @@
         <v>2.0830000000000002</v>
       </c>
     </row>
-    <row r="133" spans="1:48">
+    <row r="133" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>90</v>
       </c>
@@ -20984,7 +21081,7 @@
         <v>4.6520000000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:48">
+    <row r="134" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>90</v>
       </c>
@@ -21130,7 +21227,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:48">
+    <row r="135" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>95</v>
       </c>
@@ -21276,7 +21373,7 @@
         <v>25.068999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:48">
+    <row r="136" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>95</v>
       </c>
@@ -21422,7 +21519,7 @@
         <v>10.801</v>
       </c>
     </row>
-    <row r="137" spans="1:48">
+    <row r="137" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>95</v>
       </c>
@@ -21568,7 +21665,7 @@
         <v>6.0869999999999997</v>
       </c>
     </row>
-    <row r="138" spans="1:48">
+    <row r="138" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>95</v>
       </c>
@@ -21714,7 +21811,7 @@
         <v>6.2089999999999996</v>
       </c>
     </row>
-    <row r="139" spans="1:48">
+    <row r="139" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>95</v>
       </c>
@@ -21860,7 +21957,7 @@
         <v>2.109</v>
       </c>
     </row>
-    <row r="140" spans="1:48">
+    <row r="140" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>95</v>
       </c>
@@ -22006,7 +22103,7 @@
         <v>4.242</v>
       </c>
     </row>
-    <row r="141" spans="1:48">
+    <row r="141" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>95</v>
       </c>
@@ -22152,7 +22249,7 @@
         <v>0.41799999999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:48">
+    <row r="142" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>100</v>
       </c>
@@ -22298,7 +22395,7 @@
         <v>74.617000000000004</v>
       </c>
     </row>
-    <row r="143" spans="1:48">
+    <row r="143" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>100</v>
       </c>
@@ -22444,7 +22541,7 @@
         <v>53.31</v>
       </c>
     </row>
-    <row r="144" spans="1:48">
+    <row r="144" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>100</v>
       </c>
@@ -22590,7 +22687,7 @@
         <v>17.527999999999999</v>
       </c>
     </row>
-    <row r="145" spans="1:48">
+    <row r="145" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>100</v>
       </c>
@@ -22736,7 +22833,7 @@
         <v>7.6109999999999998</v>
       </c>
     </row>
-    <row r="146" spans="1:48">
+    <row r="146" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>100</v>
       </c>
@@ -22882,7 +22979,7 @@
         <v>3.613</v>
       </c>
     </row>
-    <row r="147" spans="1:48">
+    <row r="147" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>100</v>
       </c>
@@ -23028,7 +23125,7 @@
         <v>10.417</v>
       </c>
     </row>
-    <row r="148" spans="1:48">
+    <row r="148" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>100</v>
       </c>

</xml_diff>